<commit_message>
Card Control System Design
I began the task of figuring out how the cards will be parsed, tracked,
and dispersed throughout the game.
</commit_message>
<xml_diff>
--- a/Software Engineering/Software Design Database.xlsx
+++ b/Software Engineering/Software Design Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\git\conquer\Software Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FAB7D3-9ADE-447D-9170-62D2EDAFCAC0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E85C0C-A78A-4554-82F4-560D7A044B7C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{1A2E4C4A-9748-44D0-A38A-68F42E990A22}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>idx</t>
   </si>
@@ -48,12 +48,6 @@
     <t>action</t>
   </si>
   <si>
-    <t>x;kvjc</t>
-  </si>
-  <si>
-    <t>asf</t>
-  </si>
-  <si>
     <t>solar</t>
   </si>
   <si>
@@ -67,6 +61,18 @@
   </si>
   <si>
     <t>sub_type</t>
+  </si>
+  <si>
+    <t>Snowmagdon</t>
+  </si>
+  <si>
+    <t>Let is snow!</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>weather</t>
   </si>
 </sst>
 </file>
@@ -465,7 +471,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -477,10 +483,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -490,11 +496,14 @@
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2">
         <v>-100</v>
@@ -502,13 +511,13 @@
       <c r="G2" s="4">
         <v>0.5</v>
       </c>
-      <c r="H2" s="4">
-        <v>0.1</v>
+      <c r="H2" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" s="2">
         <v>500</v>
@@ -516,7 +525,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued Work on Card Management
I continued to work on the card management system and started to
finalized the layout of the CSV database.
</commit_message>
<xml_diff>
--- a/Software Engineering/Software Design Database.xlsx
+++ b/Software Engineering/Software Design Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\git\conquer\Software Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E85C0C-A78A-4554-82F4-560D7A044B7C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAACADA-57B3-4CCB-98FC-5A1CFB099869}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{1A2E4C4A-9748-44D0-A38A-68F42E990A22}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>idx</t>
   </si>
@@ -54,12 +54,6 @@
     <t>planet</t>
   </si>
   <si>
-    <t>defacto</t>
-  </si>
-  <si>
-    <t>range</t>
-  </si>
-  <si>
     <t>sub_type</t>
   </si>
   <si>
@@ -73,6 +67,30 @@
   </si>
   <si>
     <t>weather</t>
+  </si>
+  <si>
+    <t>Ocotpi</t>
+  </si>
+  <si>
+    <t>We are an allien race of octopi!</t>
+  </si>
+  <si>
+    <t>pop_change_rate</t>
+  </si>
+  <si>
+    <t>Ice System 1</t>
+  </si>
+  <si>
+    <t>We like ice in our solar system:)</t>
+  </si>
+  <si>
+    <t>action_type_percent_rate</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>We are human.</t>
   </si>
 </sst>
 </file>
@@ -443,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC48EAE-2AED-493D-9D4C-EB85A8518192}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -454,10 +472,11 @@
     <col min="1" max="1" width="13.44140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="2"/>
     <col min="3" max="3" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="15.44140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="14" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" style="2" customWidth="1"/>
-    <col min="7" max="8" width="13.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="29.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.21875" style="4" customWidth="1"/>
     <col min="9" max="9" width="17.77734375" style="2" customWidth="1"/>
     <col min="10" max="10" width="17.5546875" style="2" customWidth="1"/>
     <col min="11" max="16384" width="8.88671875" style="2"/>
@@ -471,7 +490,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -483,10 +502,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -497,35 +516,91 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2">
         <v>-100</v>
       </c>
-      <c r="G2" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>14</v>
+      <c r="G2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="F3" s="2">
-        <v>500</v>
+        <v>300</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2">
+        <v>500</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B5" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="2">
+        <v>600</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued work on the card drawing system
I got the most of the planet and solar system card drawing working.
</commit_message>
<xml_diff>
--- a/Software Engineering/Software Design Database.xlsx
+++ b/Software Engineering/Software Design Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\git\conquer\Software Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEDA08F-F9BF-4B00-BE09-2C3DF9AD71C3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06742D15-8786-4763-9C28-3B1A92E280CF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{1A2E4C4A-9748-44D0-A38A-68F42E990A22}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>idx</t>
   </si>
@@ -103,6 +103,24 @@
   </si>
   <si>
     <t>images/earth.jpg</t>
+  </si>
+  <si>
+    <t>Norman</t>
+  </si>
+  <si>
+    <t>MOOOOO!</t>
+  </si>
+  <si>
+    <t>images/norman.jpg</t>
+  </si>
+  <si>
+    <t>Mars</t>
+  </si>
+  <si>
+    <t>We will conquer the entire galaxy!!!</t>
+  </si>
+  <si>
+    <t>images/mars.jpg</t>
   </si>
 </sst>
 </file>
@@ -473,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC48EAE-2AED-493D-9D4C-EB85A8518192}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -639,6 +657,64 @@
         <v>25</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="2">
+        <v>999</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.04</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="2">
+        <v>100000</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added the solar system cards to the file.
</commit_message>
<xml_diff>
--- a/Software Engineering/Software Design Database.xlsx
+++ b/Software Engineering/Software Design Database.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\git\conquer\Software Engineering\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720020C0-E9C5-4EDC-9323-EBDD2D31730D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{1A2E4C4A-9748-44D0-A38A-68F42E990A22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t>idx</t>
   </si>
@@ -124,12 +118,66 @@
   </si>
   <si>
     <t>image_location*</t>
+  </si>
+  <si>
+    <t>Spartis System</t>
+  </si>
+  <si>
+    <t>Spartis the name, Technology's the game</t>
+  </si>
+  <si>
+    <t>images/Spartis System.png</t>
+  </si>
+  <si>
+    <t>Parcivel System</t>
+  </si>
+  <si>
+    <t>Why have peace when you can have war?</t>
+  </si>
+  <si>
+    <t>images/Parcivel System.png</t>
+  </si>
+  <si>
+    <t>Lightness System</t>
+  </si>
+  <si>
+    <t>images/Lightness System.png</t>
+  </si>
+  <si>
+    <t>Leafor System</t>
+  </si>
+  <si>
+    <t>Just keep those inferier races out our our space</t>
+  </si>
+  <si>
+    <t>Life is the most precious thing around here</t>
+  </si>
+  <si>
+    <t>images/Leafor System.png</t>
+  </si>
+  <si>
+    <t>Garval System</t>
+  </si>
+  <si>
+    <t>images/Garval System.png</t>
+  </si>
+  <si>
+    <t>Everything you do is for the homeworld</t>
+  </si>
+  <si>
+    <t>Bargeme System</t>
+  </si>
+  <si>
+    <t>images/Bargeme System.png</t>
+  </si>
+  <si>
+    <t>Everyone should have government issued land</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -486,36 +534,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC48EAE-2AED-493D-9D4C-EB85A8518192}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="13.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="2"/>
     <col min="3" max="3" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="14" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="29.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.21875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="25.88671875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17.5546875" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="2"/>
+    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,7 +595,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -579,7 +627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -611,7 +659,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -643,7 +691,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -675,7 +723,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -707,7 +755,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -739,147 +787,219 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Added 21 new cards to the database
</commit_message>
<xml_diff>
--- a/Software Engineering/Software Design Database.xlsx
+++ b/Software Engineering/Software Design Database.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="114">
   <si>
     <t>idx</t>
   </si>
@@ -172,6 +172,195 @@
   </si>
   <si>
     <t>Everyone should have government issued land</t>
+  </si>
+  <si>
+    <t>Black Hole</t>
+  </si>
+  <si>
+    <t>images/Black Hole.png</t>
+  </si>
+  <si>
+    <t>At least something takes care of the garbage in the universe</t>
+  </si>
+  <si>
+    <t>Core Drilling Explosion</t>
+  </si>
+  <si>
+    <t>I guess you mined a little too much</t>
+  </si>
+  <si>
+    <t>images/Core Drilling Explosion.png</t>
+  </si>
+  <si>
+    <t>Dead Planet</t>
+  </si>
+  <si>
+    <t>Life just disappeared</t>
+  </si>
+  <si>
+    <t>images/Dead Planet.png</t>
+  </si>
+  <si>
+    <t>Fire Storm</t>
+  </si>
+  <si>
+    <t>Save the trees</t>
+  </si>
+  <si>
+    <t>images/Fire Storm.png</t>
+  </si>
+  <si>
+    <t>gas hurricane</t>
+  </si>
+  <si>
+    <t>As long as you are not near this thing, you will be fine</t>
+  </si>
+  <si>
+    <t>images/gas hurricane.png</t>
+  </si>
+  <si>
+    <t>Hard Baked</t>
+  </si>
+  <si>
+    <t>Try not to waste too much water</t>
+  </si>
+  <si>
+    <t>images/Hard Baked.png</t>
+  </si>
+  <si>
+    <t>Ice Age</t>
+  </si>
+  <si>
+    <t>Everyone there are cold hearted</t>
+  </si>
+  <si>
+    <t>images/Ice Age.png</t>
+  </si>
+  <si>
+    <t>Lighting Storm</t>
+  </si>
+  <si>
+    <t>Magnetic storms can get nasty</t>
+  </si>
+  <si>
+    <t>images/Lighting Storm.png</t>
+  </si>
+  <si>
+    <t>Nucular Explosion</t>
+  </si>
+  <si>
+    <t>images/Nucular Explosion.png</t>
+  </si>
+  <si>
+    <t>Nucular power is the best way to get energy</t>
+  </si>
+  <si>
+    <t>Nucular Fission</t>
+  </si>
+  <si>
+    <t>images/Nucular Fission.png</t>
+  </si>
+  <si>
+    <t>Your planet became a star, now there's energy</t>
+  </si>
+  <si>
+    <t>Over Exposure</t>
+  </si>
+  <si>
+    <t>One to many trips close to the star</t>
+  </si>
+  <si>
+    <t>images/Over Exposure.png</t>
+  </si>
+  <si>
+    <t>Plasma Fire</t>
+  </si>
+  <si>
+    <t>Have fun trying to put this one out</t>
+  </si>
+  <si>
+    <t>images/Plasma Fire.png</t>
+  </si>
+  <si>
+    <t>Super Iodine Explosion</t>
+  </si>
+  <si>
+    <t>Iodide explosives gone wrong</t>
+  </si>
+  <si>
+    <t>imager/Super Iodine Explosion.png</t>
+  </si>
+  <si>
+    <t>Super Nova</t>
+  </si>
+  <si>
+    <t>Lots and lots of energy</t>
+  </si>
+  <si>
+    <t>images/Super Nova.png</t>
+  </si>
+  <si>
+    <t>Super Novo</t>
+  </si>
+  <si>
+    <t>Am I drunk, of is the air on fire?</t>
+  </si>
+  <si>
+    <t>images/Super Novo.png</t>
+  </si>
+  <si>
+    <t>Time Explosion</t>
+  </si>
+  <si>
+    <t>images/Time Explosion.png</t>
+  </si>
+  <si>
+    <t>How strange, that explosion seemed to have happened in the future...</t>
+  </si>
+  <si>
+    <t>Total Core Meltdown</t>
+  </si>
+  <si>
+    <t>Too much lava, not enough rock</t>
+  </si>
+  <si>
+    <t>images/Total Core Meltdown.png</t>
+  </si>
+  <si>
+    <t>Planet Gregren</t>
+  </si>
+  <si>
+    <t>images/Planet Gregren.png</t>
+  </si>
+  <si>
+    <t>Known for its high amount of gasses</t>
+  </si>
+  <si>
+    <t>Planet Lightner</t>
+  </si>
+  <si>
+    <t>Perfect place for a colony</t>
+  </si>
+  <si>
+    <t>images/Planet Lightner.png</t>
+  </si>
+  <si>
+    <t>Planet Narges</t>
+  </si>
+  <si>
+    <t>A bit cold, but has a great light show</t>
+  </si>
+  <si>
+    <t>images/Planet Narges.png</t>
+  </si>
+  <si>
+    <t>Planet Sistene</t>
+  </si>
+  <si>
+    <t>Named for its heavenly look</t>
+  </si>
+  <si>
+    <t>images/Planet Sistene.png</t>
   </si>
 </sst>
 </file>
@@ -534,7 +723,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -542,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -904,104 +1093,360 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed spaces on cards
</commit_message>
<xml_diff>
--- a/Software Engineering/Software Design Database.xlsx
+++ b/Software Engineering/Software Design Database.xlsx
@@ -723,7 +723,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -731,15 +731,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7" style="2" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" style="2"/>
     <col min="3" max="3" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" style="2" customWidth="1"/>
@@ -1092,6 +1092,18 @@
       <c r="A16" s="2">
         <v>15</v>
       </c>
+      <c r="B16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
@@ -1101,13 +1113,13 @@
         <v>2</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.35">
@@ -1118,13 +1130,13 @@
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1135,13 +1147,13 @@
         <v>2</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1152,13 +1164,13 @@
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1169,13 +1181,13 @@
         <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1186,13 +1198,13 @@
         <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -1203,13 +1215,13 @@
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -1220,13 +1232,13 @@
         <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -1237,13 +1249,13 @@
         <v>2</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1254,13 +1266,13 @@
         <v>2</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1271,13 +1283,13 @@
         <v>2</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1288,13 +1300,13 @@
         <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1305,13 +1317,13 @@
         <v>2</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -1322,13 +1334,13 @@
         <v>2</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -1339,13 +1351,13 @@
         <v>2</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -1356,13 +1368,13 @@
         <v>2</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -1370,22 +1382,34 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
+      <c r="B34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
@@ -1395,13 +1419,13 @@
         <v>4</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -1412,40 +1436,12 @@
         <v>4</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B37" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I38" s="2" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed DB and removed serialized ids'
</commit_message>
<xml_diff>
--- a/Software Engineering/Software Design Database.xlsx
+++ b/Software Engineering/Software Design Database.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\git\conquer\Software Engineering\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D41A6DF-1961-4145-B721-7D2E2EE22F6E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="94">
   <si>
     <t>idx</t>
   </si>
@@ -39,72 +45,12 @@
     <t>sub_type</t>
   </si>
   <si>
-    <t>Snowmagdon</t>
-  </si>
-  <si>
-    <t>Let is snow!</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>weather</t>
-  </si>
-  <si>
-    <t>Ocotpi</t>
-  </si>
-  <si>
-    <t>We are an allien race of octopi!</t>
-  </si>
-  <si>
     <t>pop_change_rate</t>
   </si>
   <si>
-    <t>Ice System 1</t>
-  </si>
-  <si>
-    <t>We like ice in our solar system:)</t>
-  </si>
-  <si>
     <t>action_type_percent_rate</t>
   </si>
   <si>
-    <t>Earth</t>
-  </si>
-  <si>
-    <t>We are human.</t>
-  </si>
-  <si>
-    <t>images/snow.jpg</t>
-  </si>
-  <si>
-    <t>images/ice_system.jpg</t>
-  </si>
-  <si>
-    <t>images/octopus.png</t>
-  </si>
-  <si>
-    <t>images/earth.jpg</t>
-  </si>
-  <si>
-    <t>Norman</t>
-  </si>
-  <si>
-    <t>MOOOOO!</t>
-  </si>
-  <si>
-    <t>images/norman.jpg</t>
-  </si>
-  <si>
-    <t>Mars</t>
-  </si>
-  <si>
-    <t>We will conquer the entire galaxy!!!</t>
-  </si>
-  <si>
-    <t>images/mars.jpg</t>
-  </si>
-  <si>
     <t>rource_count</t>
   </si>
   <si>
@@ -126,24 +72,15 @@
     <t>Spartis the name, Technology's the game</t>
   </si>
   <si>
-    <t>images/Spartis System.png</t>
-  </si>
-  <si>
     <t>Parcivel System</t>
   </si>
   <si>
     <t>Why have peace when you can have war?</t>
   </si>
   <si>
-    <t>images/Parcivel System.png</t>
-  </si>
-  <si>
     <t>Lightness System</t>
   </si>
   <si>
-    <t>images/Lightness System.png</t>
-  </si>
-  <si>
     <t>Leafor System</t>
   </si>
   <si>
@@ -153,33 +90,21 @@
     <t>Life is the most precious thing around here</t>
   </si>
   <si>
-    <t>images/Leafor System.png</t>
-  </si>
-  <si>
     <t>Garval System</t>
   </si>
   <si>
-    <t>images/Garval System.png</t>
-  </si>
-  <si>
     <t>Everything you do is for the homeworld</t>
   </si>
   <si>
     <t>Bargeme System</t>
   </si>
   <si>
-    <t>images/Bargeme System.png</t>
-  </si>
-  <si>
     <t>Everyone should have government issued land</t>
   </si>
   <si>
     <t>Black Hole</t>
   </si>
   <si>
-    <t>images/Black Hole.png</t>
-  </si>
-  <si>
     <t>At least something takes care of the garbage in the universe</t>
   </si>
   <si>
@@ -189,78 +114,51 @@
     <t>I guess you mined a little too much</t>
   </si>
   <si>
-    <t>images/Core Drilling Explosion.png</t>
-  </si>
-  <si>
     <t>Dead Planet</t>
   </si>
   <si>
     <t>Life just disappeared</t>
   </si>
   <si>
-    <t>images/Dead Planet.png</t>
-  </si>
-  <si>
     <t>Fire Storm</t>
   </si>
   <si>
     <t>Save the trees</t>
   </si>
   <si>
-    <t>images/Fire Storm.png</t>
-  </si>
-  <si>
     <t>gas hurricane</t>
   </si>
   <si>
     <t>As long as you are not near this thing, you will be fine</t>
   </si>
   <si>
-    <t>images/gas hurricane.png</t>
-  </si>
-  <si>
     <t>Hard Baked</t>
   </si>
   <si>
     <t>Try not to waste too much water</t>
   </si>
   <si>
-    <t>images/Hard Baked.png</t>
-  </si>
-  <si>
     <t>Ice Age</t>
   </si>
   <si>
     <t>Everyone there are cold hearted</t>
   </si>
   <si>
-    <t>images/Ice Age.png</t>
-  </si>
-  <si>
     <t>Lighting Storm</t>
   </si>
   <si>
     <t>Magnetic storms can get nasty</t>
   </si>
   <si>
-    <t>images/Lighting Storm.png</t>
-  </si>
-  <si>
     <t>Nucular Explosion</t>
   </si>
   <si>
-    <t>images/Nucular Explosion.png</t>
-  </si>
-  <si>
     <t>Nucular power is the best way to get energy</t>
   </si>
   <si>
     <t>Nucular Fission</t>
   </si>
   <si>
-    <t>images/Nucular Fission.png</t>
-  </si>
-  <si>
     <t>Your planet became a star, now there's energy</t>
   </si>
   <si>
@@ -270,18 +168,12 @@
     <t>One to many trips close to the star</t>
   </si>
   <si>
-    <t>images/Over Exposure.png</t>
-  </si>
-  <si>
     <t>Plasma Fire</t>
   </si>
   <si>
     <t>Have fun trying to put this one out</t>
   </si>
   <si>
-    <t>images/Plasma Fire.png</t>
-  </si>
-  <si>
     <t>Super Iodine Explosion</t>
   </si>
   <si>
@@ -297,24 +189,15 @@
     <t>Lots and lots of energy</t>
   </si>
   <si>
-    <t>images/Super Nova.png</t>
-  </si>
-  <si>
     <t>Super Novo</t>
   </si>
   <si>
     <t>Am I drunk, of is the air on fire?</t>
   </si>
   <si>
-    <t>images/Super Novo.png</t>
-  </si>
-  <si>
     <t>Time Explosion</t>
   </si>
   <si>
-    <t>images/Time Explosion.png</t>
-  </si>
-  <si>
     <t>How strange, that explosion seemed to have happened in the future...</t>
   </si>
   <si>
@@ -324,15 +207,9 @@
     <t>Too much lava, not enough rock</t>
   </si>
   <si>
-    <t>images/Total Core Meltdown.png</t>
-  </si>
-  <si>
     <t>Planet Gregren</t>
   </si>
   <si>
-    <t>images/Planet Gregren.png</t>
-  </si>
-  <si>
     <t>Known for its high amount of gasses</t>
   </si>
   <si>
@@ -342,31 +219,100 @@
     <t>Perfect place for a colony</t>
   </si>
   <si>
-    <t>images/Planet Lightner.png</t>
-  </si>
-  <si>
     <t>Planet Narges</t>
   </si>
   <si>
     <t>A bit cold, but has a great light show</t>
   </si>
   <si>
-    <t>images/Planet Narges.png</t>
-  </si>
-  <si>
     <t>Planet Sistene</t>
   </si>
   <si>
     <t>Named for its heavenly look</t>
   </si>
   <si>
-    <t>images/Planet Sistene.png</t>
+    <t>Spartis System.png</t>
+  </si>
+  <si>
+    <t>Parcivel System.png</t>
+  </si>
+  <si>
+    <t>Lightness System.png</t>
+  </si>
+  <si>
+    <t>Leafor System.png</t>
+  </si>
+  <si>
+    <t>Garval System.png</t>
+  </si>
+  <si>
+    <t>Bargeme System.png</t>
+  </si>
+  <si>
+    <t>Black Hole.png</t>
+  </si>
+  <si>
+    <t>Core Drilling Explosion.png</t>
+  </si>
+  <si>
+    <t>Dead Planet.png</t>
+  </si>
+  <si>
+    <t>Fire Storm.png</t>
+  </si>
+  <si>
+    <t>gas hurricane.png</t>
+  </si>
+  <si>
+    <t>Hard Baked.png</t>
+  </si>
+  <si>
+    <t>Ice Age.png</t>
+  </si>
+  <si>
+    <t>Lighting Storm.png</t>
+  </si>
+  <si>
+    <t>Nucular Explosion.png</t>
+  </si>
+  <si>
+    <t>Nucular Fission.png</t>
+  </si>
+  <si>
+    <t>Over Exposure.png</t>
+  </si>
+  <si>
+    <t>Plasma Fire.png</t>
+  </si>
+  <si>
+    <t>Super Nova.png</t>
+  </si>
+  <si>
+    <t>Super Novo.png</t>
+  </si>
+  <si>
+    <t>Time Explosion.png</t>
+  </si>
+  <si>
+    <t>Total Core Meltdown.png</t>
+  </si>
+  <si>
+    <t>Planet Gregren.png</t>
+  </si>
+  <si>
+    <t>Planet Lightner.png</t>
+  </si>
+  <si>
+    <t>Planet Narges.png</t>
+  </si>
+  <si>
+    <t>Planet Sistene.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -723,372 +669,306 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="8.88671875" style="2"/>
     <col min="3" max="3" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="14" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="2"/>
+    <col min="6" max="6" width="13.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="29.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="30.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2">
-        <v>-100</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="4">
-        <v>0.3</v>
+        <v>14</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="2">
-        <v>300</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0.3</v>
+        <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2">
-        <v>500</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0.2</v>
+        <v>19</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="2">
-        <v>600</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="4">
-        <v>0.03</v>
+        <v>20</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="2">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="2">
-        <v>999</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0.04</v>
+        <v>22</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="2">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="2">
-        <v>100000</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="4">
-        <v>0.5</v>
+        <v>24</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="2">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1096,16 +976,16 @@
         <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1113,16 +993,16 @@
         <v>2</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1130,16 +1010,16 @@
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1147,16 +1027,16 @@
         <v>2</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1164,16 +1044,16 @@
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1181,16 +1061,16 @@
         <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1198,16 +1078,16 @@
         <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1215,16 +1095,16 @@
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1232,217 +1112,81 @@
         <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>28</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>29</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <v>30</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
-        <v>31</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
-        <v>32</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
-        <v>33</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
-        <v>34</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
-        <v>35</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cosmetic Changes and New Cards.
I made a bunch of little cosmetic changes especially to the fight modal,
and I implemented the new cards for the game.
</commit_message>
<xml_diff>
--- a/Software Engineering/Software Design Database.xlsx
+++ b/Software Engineering/Software Design Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\git\conquer\Software Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D41A6DF-1961-4145-B721-7D2E2EE22F6E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A88B552-9DAB-494F-829D-7CAFB9031655}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="95">
   <si>
     <t>idx</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Spartis System</t>
   </si>
   <si>
-    <t>Spartis the name, Technology's the game</t>
-  </si>
-  <si>
     <t>Parcivel System</t>
   </si>
   <si>
@@ -180,9 +177,6 @@
     <t>Iodide explosives gone wrong</t>
   </si>
   <si>
-    <t>imager/Super Iodine Explosion.png</t>
-  </si>
-  <si>
     <t>Super Nova</t>
   </si>
   <si>
@@ -307,6 +301,15 @@
   </si>
   <si>
     <t>Planet Sistene.png</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Super Iodine Explosion.png</t>
+  </si>
+  <si>
+    <t>Spartis the name, Technologys the game</t>
   </si>
 </sst>
 </file>
@@ -679,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -689,7 +692,7 @@
     <col min="2" max="2" width="8.88671875" style="2"/>
     <col min="3" max="3" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="29.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.33203125" style="4" customWidth="1"/>
@@ -737,14 +740,29 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>94</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0.03</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="J2" s="2">
+        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -754,14 +772,29 @@
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.03</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="J3" s="2">
+        <v>500</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -771,14 +804,29 @@
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.03</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="J4" s="2">
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -788,14 +836,29 @@
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.03</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
+      </c>
+      <c r="J5" s="2">
+        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -805,14 +868,29 @@
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>22</v>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.03</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+      <c r="J6" s="2">
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -822,14 +900,29 @@
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>24</v>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.03</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
+      </c>
+      <c r="J7" s="2">
+        <v>500</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -839,14 +932,29 @@
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>26</v>
+      <c r="F8" s="2">
+        <v>-500</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0.03</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -856,14 +964,29 @@
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>28</v>
+      <c r="F9" s="2">
+        <v>-500</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.03</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -873,14 +996,29 @@
       <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C10" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>30</v>
+      <c r="F10" s="2">
+        <v>-500</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.03</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -890,14 +1028,29 @@
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>32</v>
+      <c r="F11" s="2">
+        <v>-500</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.03</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -907,14 +1060,29 @@
       <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C12" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>34</v>
+      <c r="F12" s="2">
+        <v>-500</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.03</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -924,14 +1092,29 @@
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C13" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>36</v>
+      <c r="F13" s="2">
+        <v>-500</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0.03</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -941,14 +1124,29 @@
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C14" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>38</v>
+      <c r="F14" s="2">
+        <v>-500</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0.03</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -958,14 +1156,29 @@
       <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>40</v>
+      <c r="F15" s="2">
+        <v>-500</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0.03</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -975,218 +1188,413 @@
       <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C16" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>42</v>
+      <c r="F16" s="2">
+        <v>-500</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0.03</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C17" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>44</v>
+      <c r="F17" s="2">
+        <v>-500</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0.03</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C18" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>46</v>
+      <c r="F18" s="2">
+        <v>-500</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0.03</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C19" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>48</v>
+      <c r="F19" s="2">
+        <v>-500</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0.03</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C20" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>50</v>
+      <c r="F20" s="2">
+        <v>-500</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0.03</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C21" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D21" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="F21" s="2">
+        <v>-500</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0.03</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C22" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D22" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="F22" s="2">
+        <v>-500</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0.03</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C23" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D23" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="F23" s="2">
+        <v>-500</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0.03</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C24" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D24" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="F24" s="2">
+        <v>600</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0.03</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C25" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D25" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="F25" s="2">
+        <v>500</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0.03</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+      <c r="J25" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C26" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D26" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="F26" s="2">
+        <v>600</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0.03</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+      <c r="J26" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C27" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D27" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="F27" s="2">
+        <v>500</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0.03</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+      <c r="J27" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C28" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="D28" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="F28" s="2">
+        <v>600</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0.03</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
+      </c>
+      <c r="J28" s="2">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 11 new planet cards.
</commit_message>
<xml_diff>
--- a/Software Engineering/Software Design Database.xlsx
+++ b/Software Engineering/Software Design Database.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="153">
   <si>
     <t>idx</t>
   </si>
@@ -304,6 +304,180 @@
   </si>
   <si>
     <t>Am I drunk, or is the air on fire?</t>
+  </si>
+  <si>
+    <t>Planet Acere</t>
+  </si>
+  <si>
+    <t>Planet Acere.png</t>
+  </si>
+  <si>
+    <t>Planet Carbonic</t>
+  </si>
+  <si>
+    <t>Planet Carbonic.png</t>
+  </si>
+  <si>
+    <t>Planet East Eggor</t>
+  </si>
+  <si>
+    <t>Planet East Eggor.png</t>
+  </si>
+  <si>
+    <t>Planet Eden</t>
+  </si>
+  <si>
+    <t>Planet Eden.png</t>
+  </si>
+  <si>
+    <t>Planet Fetlink</t>
+  </si>
+  <si>
+    <t>Planet Fetlink.png</t>
+  </si>
+  <si>
+    <t>Planet Garbonic</t>
+  </si>
+  <si>
+    <t>Planet Garbonic.png</t>
+  </si>
+  <si>
+    <t>Planet Hearon</t>
+  </si>
+  <si>
+    <t>Planet Hearon.png</t>
+  </si>
+  <si>
+    <t>Planet Hogsworth</t>
+  </si>
+  <si>
+    <t>Planet Hogsworth.png</t>
+  </si>
+  <si>
+    <t>Planet Ikeness</t>
+  </si>
+  <si>
+    <t>Planet Ikeness.png</t>
+  </si>
+  <si>
+    <t>Planet Mitter</t>
+  </si>
+  <si>
+    <t>Planet Mitter.png</t>
+  </si>
+  <si>
+    <t>Planet Napaul</t>
+  </si>
+  <si>
+    <t>Planet Napaul.png</t>
+  </si>
+  <si>
+    <t>Planet Networth</t>
+  </si>
+  <si>
+    <t>Planet Networth.png</t>
+  </si>
+  <si>
+    <t>Planet Pluton</t>
+  </si>
+  <si>
+    <t>Planet Pluton.png</t>
+  </si>
+  <si>
+    <t>Planet Satiron</t>
+  </si>
+  <si>
+    <t>Planet Satiron.png</t>
+  </si>
+  <si>
+    <t>Planet Scysm</t>
+  </si>
+  <si>
+    <t>Planet Scysm.png</t>
+  </si>
+  <si>
+    <t>Planet Starstir</t>
+  </si>
+  <si>
+    <t>Planet Starstir.png</t>
+  </si>
+  <si>
+    <t>Planet Telepan</t>
+  </si>
+  <si>
+    <t>Planet Telepan.png</t>
+  </si>
+  <si>
+    <t>Planet Zastron</t>
+  </si>
+  <si>
+    <t>Planet Zastron.png</t>
+  </si>
+  <si>
+    <t>Planet Zerox</t>
+  </si>
+  <si>
+    <t>Planet Zerox.png</t>
+  </si>
+  <si>
+    <t>Hearon this planet is life.</t>
+  </si>
+  <si>
+    <t>I looks pink from space, but on the surface it is all red</t>
+  </si>
+  <si>
+    <t>Look at all the carbon in the atmosphere</t>
+  </si>
+  <si>
+    <t>I hope there is water somewhere on the surface</t>
+  </si>
+  <si>
+    <t>Secret weapon</t>
+  </si>
+  <si>
+    <t>The perfect place to add to the empire's trophies</t>
+  </si>
+  <si>
+    <t>Mostly covered in lava. Just be careful</t>
+  </si>
+  <si>
+    <t>There is snow all over this planet</t>
+  </si>
+  <si>
+    <t>A very old planet, but it will do the job</t>
+  </si>
+  <si>
+    <t>Named for its ink like look</t>
+  </si>
+  <si>
+    <t>Comes with a built in belt</t>
+  </si>
+  <si>
+    <t>Has excess of oxygen everywhere</t>
+  </si>
+  <si>
+    <t>Has a built in planetary defence system</t>
+  </si>
+  <si>
+    <t>Rumored to have Plutonium at its core</t>
+  </si>
+  <si>
+    <t>Semi-transparent planet</t>
+  </si>
+  <si>
+    <t>It has its own moon, have fun</t>
+  </si>
+  <si>
+    <t>Glows from space. Hopefully it is  gold</t>
+  </si>
+  <si>
+    <t>A few gas storms, but nothing our shields can't handle</t>
+  </si>
+  <si>
+    <t>Just a big rock. Hopefully the core is usable</t>
+  </si>
+  <si>
+    <t>A very nice planet</t>
   </si>
 </sst>
 </file>
@@ -666,7 +840,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -674,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1591,6 +1765,332 @@
         <v>300</v>
       </c>
     </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Card drawing bug fixes
I fixed to bugs. The first one was that the background of any "cloned"
cards was only displaying the description. The second one involved
Action cards not being returned from the getSubTypeCard() in the
TurnControl class
</commit_message>
<xml_diff>
--- a/Software Engineering/Software Design Database.xlsx
+++ b/Software Engineering/Software Design Database.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\git\conquer\Software Engineering\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA9AEDC-8956-43F0-90DB-009835ECE903}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -309,7 +315,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -666,33 +672,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17:F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="8.88671875" style="2"/>
     <col min="3" max="3" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="2"/>
+    <col min="4" max="4" width="19.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="29.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="30.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -936,7 +942,7 @@
         <v>25</v>
       </c>
       <c r="F8" s="2">
-        <v>-500</v>
+        <v>-1300</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>90</v>
@@ -968,7 +974,7 @@
         <v>27</v>
       </c>
       <c r="F9" s="2">
-        <v>-500</v>
+        <v>-1300</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>90</v>
@@ -1000,7 +1006,7 @@
         <v>29</v>
       </c>
       <c r="F10" s="2">
-        <v>-500</v>
+        <v>-1300</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>90</v>
@@ -1032,7 +1038,7 @@
         <v>31</v>
       </c>
       <c r="F11" s="2">
-        <v>-500</v>
+        <v>-1300</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>90</v>
@@ -1064,7 +1070,7 @@
         <v>33</v>
       </c>
       <c r="F12" s="2">
-        <v>-500</v>
+        <v>-1300</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>90</v>
@@ -1096,7 +1102,7 @@
         <v>35</v>
       </c>
       <c r="F13" s="2">
-        <v>-500</v>
+        <v>-1300</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>90</v>
@@ -1128,7 +1134,7 @@
         <v>37</v>
       </c>
       <c r="F14" s="2">
-        <v>-500</v>
+        <v>-1300</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>90</v>
@@ -1160,7 +1166,7 @@
         <v>39</v>
       </c>
       <c r="F15" s="2">
-        <v>-500</v>
+        <v>-1300</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>90</v>
@@ -1192,7 +1198,7 @@
         <v>41</v>
       </c>
       <c r="F16" s="2">
-        <v>-500</v>
+        <v>-1300</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>90</v>
@@ -1224,7 +1230,7 @@
         <v>43</v>
       </c>
       <c r="F17" s="2">
-        <v>-500</v>
+        <v>-900</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>90</v>
@@ -1256,7 +1262,7 @@
         <v>45</v>
       </c>
       <c r="F18" s="2">
-        <v>-500</v>
+        <v>-900</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>90</v>
@@ -1288,7 +1294,7 @@
         <v>47</v>
       </c>
       <c r="F19" s="2">
-        <v>-500</v>
+        <v>-900</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>90</v>
@@ -1320,7 +1326,7 @@
         <v>49</v>
       </c>
       <c r="F20" s="2">
-        <v>-500</v>
+        <v>-900</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>90</v>
@@ -1352,7 +1358,7 @@
         <v>51</v>
       </c>
       <c r="F21" s="2">
-        <v>-500</v>
+        <v>-900</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>90</v>
@@ -1384,7 +1390,7 @@
         <v>94</v>
       </c>
       <c r="F22" s="2">
-        <v>-500</v>
+        <v>-900</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>90</v>
@@ -1416,7 +1422,7 @@
         <v>54</v>
       </c>
       <c r="F23" s="2">
-        <v>-500</v>
+        <v>-900</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>90</v>
@@ -1448,7 +1454,7 @@
         <v>56</v>
       </c>
       <c r="F24" s="2">
-        <v>600</v>
+        <v>6000</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>90</v>
@@ -1480,7 +1486,7 @@
         <v>57</v>
       </c>
       <c r="F25" s="2">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>90</v>
@@ -1512,7 +1518,7 @@
         <v>59</v>
       </c>
       <c r="F26" s="2">
-        <v>600</v>
+        <v>7000</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>90</v>
@@ -1544,7 +1550,7 @@
         <v>61</v>
       </c>
       <c r="F27" s="2">
-        <v>500</v>
+        <v>3000</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>90</v>
@@ -1576,7 +1582,7 @@
         <v>63</v>
       </c>
       <c r="F28" s="2">
-        <v>600</v>
+        <v>6000</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>90</v>

</xml_diff>